<commit_message>
Modified event.csv and For Event Table.xlsx
</commit_message>
<xml_diff>
--- a/documentation/miscellaneous/for Import/For Event Table.xlsx
+++ b/documentation/miscellaneous/for Import/For Event Table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\apc-softdev-it111-05\documentation\miscellaneous\for Import\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SOFTDEV\documentation\miscellaneous\for Import\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -795,7 +795,7 @@
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:R31"/>
+      <selection activeCell="A6" sqref="A6:N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>